<commit_message>
main.py upated minor changes to specifications
</commit_message>
<xml_diff>
--- a/Hardware/RPI5-Scan2Go-HAT/Functionele specificaties HAT.xlsx
+++ b/Hardware/RPI5-Scan2Go-HAT/Functionele specificaties HAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/cr_tak_student_han_nl/Documents/S8 (afstuderen)/Software+Hardware/Hardware/RPI5-Scan2Go-HAT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{471679F7-0749-465C-94AA-78C37701B0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BE44EEB-328C-40C9-8782-301ED0467545}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{471679F7-0749-465C-94AA-78C37701B0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92EF72FA-B14C-48BB-BF0F-270D2C4FA25F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4176" yWindow="2784" windowWidth="17280" windowHeight="8880" xr2:uid="{A1EA83D2-A6D0-4FF4-A387-952356D5B8E4}"/>
+    <workbookView minimized="1" xWindow="3768" yWindow="3768" windowWidth="17280" windowHeight="9960" xr2:uid="{A1EA83D2-A6D0-4FF4-A387-952356D5B8E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -98,133 +98,133 @@
     <t>Specificatie</t>
   </si>
   <si>
-    <t>De te ontwerpen printplaat dient de RPI PICO en de RPI elektrisch te verbinden met elkaar en de randapparatuur voor de FDS.</t>
-  </si>
-  <si>
-    <t>De printplaat moet het gebruik van de huidige breadboard opstelling overbodig maken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afmetingen van printplaat streven naar de standaard HAT formaat voor de RPI* </t>
-  </si>
-  <si>
-    <t>Alleen de front CU layer van de printplaat mag elektrische componenten bevatten</t>
-  </si>
-  <si>
-    <t>De HAT kan op de RPI(5) worden geïnstalleerd door middel van pin headers en is dus ook afneembaar</t>
-  </si>
-  <si>
     <t>F2.5</t>
   </si>
   <si>
-    <t>De elektronica moet zo plat mogelijk worden gemaakt zodat het mogelijk achter een beeldscherm kan worden geplaatst</t>
-  </si>
-  <si>
-    <t>Het bordje heeft uitgangen/poorten naar de randapparatuur</t>
-  </si>
-  <si>
-    <t>De connectoren dienen gekozen te worden naar beschikbaarheid en functionaliteit</t>
-  </si>
-  <si>
     <t>F3.2</t>
   </si>
   <si>
-    <t>Een standaard aansluiting voor audio apparatuur (speakers) is gewenst</t>
-  </si>
-  <si>
     <t>F3.3</t>
   </si>
   <si>
-    <t>Overgebleven pinnen op de PICO en RPI worden beschikbaar gesteld via connectoren.</t>
-  </si>
-  <si>
     <t>F3.4</t>
   </si>
   <si>
-    <t xml:space="preserve">Datacommunicatie tussen PICO en RPI verloopt via de HAT </t>
-  </si>
-  <si>
     <t>F3.5</t>
   </si>
   <si>
-    <t>De RPI5 kan de Pico opnieuw opstarten</t>
-  </si>
-  <si>
     <t>F3.6</t>
   </si>
   <si>
-    <t>Poorten van Raspberry Pi 5 niet door de printplaat te worden overschreden</t>
-  </si>
-  <si>
     <t>T4.1</t>
   </si>
   <si>
-    <t>De printplaat voedt de PICO</t>
-  </si>
-  <si>
     <t>T4.2</t>
   </si>
   <si>
-    <t>De printplaat voedt de RPI</t>
-  </si>
-  <si>
     <t>F4.3</t>
   </si>
   <si>
-    <t>De printplaat voedt de mmWave sensoren</t>
-  </si>
-  <si>
     <t>F4.4</t>
   </si>
   <si>
-    <t>De printplaat voedt de voedingsheaders</t>
-  </si>
-  <si>
-    <t>De printplaat bevat randapparatuur voor test en debug doeleinden</t>
-  </si>
-  <si>
-    <t>De status indicator is de RGB LED die in het ontwerp van de FDS gebruikt wordt</t>
-  </si>
-  <si>
     <t xml:space="preserve">F5.2 </t>
   </si>
   <si>
-    <t>Een reset knop voor de PICO wordt gebruikt</t>
-  </si>
-  <si>
     <t>F5.3</t>
   </si>
   <si>
-    <t>Een gebruikersknop voor de PICO wordt gebruikt</t>
-  </si>
-  <si>
-    <t>De printplaat is te gebruiken met de RPI3B+ en RPI4</t>
-  </si>
-  <si>
     <t xml:space="preserve">F6.1 </t>
   </si>
   <si>
-    <t>De audio pinnen zijn d.m.v. solder jumpers te verbinden met de GPIO van de RPI</t>
-  </si>
-  <si>
-    <t>De PICO kan op de HAT worden  geïnstalleerd door middel van pin headers en is dus ook afneembaar</t>
-  </si>
-  <si>
     <t>F7.1</t>
   </si>
   <si>
     <t>F7.0</t>
   </si>
   <si>
-    <t>De HAT bevat een latch om het signaal van de metaaldetector op te vangen</t>
-  </si>
-  <si>
-    <t>De latch wordt door de HAT gereset</t>
-  </si>
-  <si>
-    <t>De printplaat kan de vooraf vastgestelde randapparatuur voeden</t>
-  </si>
-  <si>
-    <t>De printplaat wordt ontworpen als een HAT voor de RPI5 waar de pico kan op worden geïnstalleerd</t>
+    <t>De printplaat moet het gebruik van de huidige breadboard opstelling overbodig maken.</t>
+  </si>
+  <si>
+    <t>Alleen de front CU layer van de printplaat mag elektrische componenten bevatten.</t>
+  </si>
+  <si>
+    <t>De elektronica moet zo plat mogelijk worden gemaakt zodat het mogelijk achter een beeldscherm kan worden geplaatst.</t>
+  </si>
+  <si>
+    <t>Het bordje heeft uitgangen/poorten naar de randapparatuur.</t>
+  </si>
+  <si>
+    <t>De connectoren dienen gekozen te worden naar beschikbaarheid en functionaliteit.</t>
+  </si>
+  <si>
+    <t>Een standaard aansluiting voor audio apparatuur (speakers) is gewenst.</t>
+  </si>
+  <si>
+    <t>De printplaat kan de vooraf vastgestelde randapparatuur voeden.</t>
+  </si>
+  <si>
+    <t>De printplaat voedt de mmWave sensoren.</t>
+  </si>
+  <si>
+    <t>De printplaat voedt de voedingsheaders.</t>
+  </si>
+  <si>
+    <t>De printplaat bevat randapparatuur voor test en debug doeleinden.</t>
+  </si>
+  <si>
+    <t>De latch wordt door de HAT gereset.</t>
+  </si>
+  <si>
+    <t>De HAT bevat een latch om het signaal van de metaaldetector op te vangen.</t>
+  </si>
+  <si>
+    <t>Afmetingen van printplaat streven naar de standaard HAT formaat voor de Raspberry Pi 5 (zie paragraaf 6.1)</t>
+  </si>
+  <si>
+    <t>De printplaat voedt de Raspberry Pi 5.</t>
+  </si>
+  <si>
+    <t>De audio pinnen zijn d.m.v. solder jumpers te verbinden met de GPIO van de Raspberry Pi 5.</t>
+  </si>
+  <si>
+    <t>De printplaat is te gebruiken met de Raspberry Pi 3B+ en Raspberry Pi 4.</t>
+  </si>
+  <si>
+    <t>De te ontwerpen printplaat dient de Raspberry Pi Pico en de Raspberry Pi 5 elektrisch te verbinden met elkaar en de randapparatuur voor de FDS.</t>
+  </si>
+  <si>
+    <t>De printplaat wordt ontworpen als een HAT voor de Raspberry Pi 5 waar de Raspberry Pi Pico kan op worden geïnstalleerd.</t>
+  </si>
+  <si>
+    <t>De Raspberry Pi Pico kan op de HAT worden  geïnstalleerd door middel van pin headers en is dus ook afneembaar.</t>
+  </si>
+  <si>
+    <t>Overgebleven pinnen op de Raspberry Pi Pico en Raspberry Pi 5 worden beschikbaar gesteld via connectoren.</t>
+  </si>
+  <si>
+    <t>Datacommunicatie tussen Raspberry Pi Pico en Raspberry Pi 5 verloopt via de HAT .</t>
+  </si>
+  <si>
+    <t>De Raspberry Pi 5 kan de Raspberry Pi Pico opnieuw opstarten.</t>
+  </si>
+  <si>
+    <t>De printplaat voedt de Raspberry Pi Pico.</t>
+  </si>
+  <si>
+    <t>Een reset knop voor de Raspberry Pi Pico wordt gebruikt.</t>
+  </si>
+  <si>
+    <t>Een gebruikersknop voor de Raspberry Pi Pico wordt gebruikt.</t>
+  </si>
+  <si>
+    <t>De HAT kan op de Raspberry Pi (5) worden geïnstalleerd door middel van pin headers en is dus ook afneembaar.</t>
+  </si>
+  <si>
+    <t>Poorten van Raspberry Pi 5 dienen niet door de printplaat te worden overschreden.</t>
+  </si>
+  <si>
+    <t>De status indicator is de RGB-LED die in het ontwerp van de FDS gebruikt wordt.</t>
   </si>
 </sst>
 </file>
@@ -267,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -286,37 +286,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -483,11 +452,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -495,79 +479,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7C3E10-E9C9-4DAC-83DF-6861CB9F2522}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="A1:C29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,340 +894,339 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C13" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="C24" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="C25" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="C26" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="C28" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="14"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="26"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>